<commit_message>
Flush out holder and holdings object use system, fix objects in place when held, NE
</commit_message>
<xml_diff>
--- a/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
+++ b/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00jul\ProjectHumans\ProjectHumans\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BBA0D7-63BC-46FB-B82E-367F8FD99C6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2AF67C-E21F-4258-97D3-36FBBF974A3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-72" yWindow="180" windowWidth="23040" windowHeight="11460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old" sheetId="1" r:id="rId1"/>
     <sheet name="AI" sheetId="2" r:id="rId2"/>
+    <sheet name="Motor" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="175">
   <si>
     <t>System</t>
   </si>
@@ -345,13 +346,370 @@
   </si>
   <si>
     <t>Updated March 2</t>
+  </si>
+  <si>
+    <t>GetAction</t>
+  </si>
+  <si>
+    <t>string currentAction</t>
+  </si>
+  <si>
+    <t>lay down</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>consume or search</t>
+  </si>
+  <si>
+    <t>stand</t>
+  </si>
+  <si>
+    <t>move randomly</t>
+  </si>
+  <si>
+    <t>sets target and pickup, or moves to object</t>
+  </si>
+  <si>
+    <t>look for objects and explore</t>
+  </si>
+  <si>
+    <t>walks</t>
+  </si>
+  <si>
+    <t>rotates in correct direction</t>
+  </si>
+  <si>
+    <t>returns true</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>thisBody</t>
+  </si>
+  <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>stateLabelList</t>
+  </si>
+  <si>
+    <t>stateIndexDict</t>
+  </si>
+  <si>
+    <t>stateDict</t>
+  </si>
+  <si>
+    <t>args</t>
+  </si>
+  <si>
+    <t>argsLabelList</t>
+  </si>
+  <si>
+    <t>argsIndexDict</t>
+  </si>
+  <si>
+    <t>argsDict</t>
+  </si>
+  <si>
+    <t>actionList</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>Get/Set</t>
+  </si>
+  <si>
+    <t>InitStates</t>
+  </si>
+  <si>
+    <t>InitActionArguments</t>
+  </si>
+  <si>
+    <t>InitActionDict</t>
+  </si>
+  <si>
+    <t>TakeAction</t>
+  </si>
+  <si>
+    <t>int[] toDoList</t>
+  </si>
+  <si>
+    <t>PrimateMotor</t>
+  </si>
+  <si>
+    <t>public abstract</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>LookAt</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>BendWaist</t>
+  </si>
+  <si>
+    <t>float degree</t>
+  </si>
+  <si>
+    <t>BendKnees</t>
+  </si>
+  <si>
+    <t>float degree, float z</t>
+  </si>
+  <si>
+    <t>Collapse</t>
+  </si>
+  <si>
+    <t>do nothing</t>
+  </si>
+  <si>
+    <t>open eyes, no longer sleeping</t>
+  </si>
+  <si>
+    <t>fall to ground, go limp</t>
+  </si>
+  <si>
+    <t>move forward, move legs</t>
+  </si>
+  <si>
+    <t>grab item at coords</t>
+  </si>
+  <si>
+    <t>"target z"</t>
+  </si>
+  <si>
+    <t>index of active held item in body array</t>
+  </si>
+  <si>
+    <r>
+      <t>"sitting down",</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"sitting up",  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"laying down", </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"standing up", </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"rotating",    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"taking steps",</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"picking up",  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"setting down",</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 7 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"consuming",   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"waking up",   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"sleeping",    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"resting",     </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"looking"      </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 12</t>
+    </r>
+  </si>
+  <si>
+    <t>"step rate",                          </t>
+  </si>
+  <si>
+    <t>"rotation velocity",               </t>
+  </si>
+  <si>
+    <t>"held position",</t>
+  </si>
+  <si>
+    <t>"target x",</t>
+  </si>
+  <si>
+    <t>"target y",</t>
+  </si>
+  <si>
+    <t>FixItem</t>
+  </si>
+  <si>
+    <t>GO holder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -412,8 +770,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +821,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -481,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -513,6 +890,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB8D741-4165-4A5F-A7B2-A951802FB0D3}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:I13"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1402,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>36</v>
@@ -1034,93 +1417,117 @@
         <v>43</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H6" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="21" t="s">
         <v>55</v>
       </c>
       <c r="K12" s="17" t="s">
@@ -1129,9 +1536,12 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="21" t="s">
         <v>81</v>
       </c>
       <c r="K13" s="17" t="s">
@@ -1139,7 +1549,10 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J14" s="17" t="s">
+      <c r="I14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>82</v>
       </c>
       <c r="K14" s="17" t="s">
@@ -1148,9 +1561,12 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="21" t="s">
         <v>87</v>
       </c>
       <c r="K15" s="17" t="s">
@@ -1159,16 +1575,16 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="21" t="s">
         <v>78</v>
       </c>
       <c r="K18" s="17" t="s">
@@ -1180,9 +1596,9 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="21" t="s">
         <v>73</v>
       </c>
       <c r="K19" s="17" t="s">
@@ -1194,9 +1610,12 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20" s="22" t="s">
         <v>72</v>
       </c>
       <c r="K20" s="17" t="s">
@@ -1208,9 +1627,9 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="21" t="s">
         <v>67</v>
       </c>
       <c r="K21" s="17" t="s">
@@ -1221,7 +1640,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="21" t="s">
         <v>70</v>
       </c>
       <c r="K22" s="17" t="s">
@@ -1233,9 +1652,9 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="21" t="s">
         <v>76</v>
       </c>
       <c r="K23" s="17" t="s">
@@ -1247,9 +1666,9 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="21" t="s">
         <v>83</v>
       </c>
       <c r="K24" s="17" t="s">
@@ -1261,9 +1680,9 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="21" t="s">
         <v>58</v>
       </c>
       <c r="K25" s="17" t="s">
@@ -1278,6 +1697,376 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC7C482-7446-475C-85AE-DFD8793116A4}">
+  <dimension ref="A1:L37"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="15.77734375" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="J7" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="24"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="23" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add options to Help panel, fix rotation jump and gene panel display, NE
</commit_message>
<xml_diff>
--- a/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
+++ b/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00jul\ProjectHumans\ProjectHumans\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2AF67C-E21F-4258-97D3-36FBBF974A3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6302BB34-9953-4013-B583-7248B4721EBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="180" windowWidth="23040" windowHeight="11460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2544" yWindow="0" windowWidth="16752" windowHeight="12504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" r:id="rId1"/>
@@ -1709,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC7C482-7446-475C-85AE-DFD8793116A4}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1792,7 +1792,7 @@
       <c r="D5" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1806,13 +1806,13 @@
       <c r="E6" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="21" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="21" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1826,7 +1826,7 @@
       <c r="I8" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="21" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
       <c r="I14" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="21" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SitDown when called, NE
</commit_message>
<xml_diff>
--- a/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
+++ b/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00jul\ProjectHumans\ProjectHumans\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6302BB34-9953-4013-B583-7248B4721EBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C83EF-AC8D-4646-AD26-E3FE0CAF2BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="0" windowWidth="16752" windowHeight="12504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="4020" windowWidth="16752" windowHeight="12504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" r:id="rId1"/>
@@ -1710,7 +1710,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1770,7 @@
       <c r="G3" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="21" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add consume function, mouth not connected
</commit_message>
<xml_diff>
--- a/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
+++ b/ProjectHumans/Assets/Documentation/ExcelDoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00jul\ProjectHumans\ProjectHumans\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C83EF-AC8D-4646-AD26-E3FE0CAF2BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342E4928-9E73-4143-A5BF-438E0F5515DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="4020" windowWidth="16752" windowHeight="12504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="177">
   <si>
     <t>System</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>GO holder</t>
+  </si>
+  <si>
+    <t>no state update yet</t>
+  </si>
+  <si>
+    <t>not tested</t>
   </si>
 </sst>
 </file>
@@ -784,7 +790,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -827,6 +833,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -858,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -896,6 +908,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1710,7 +1723,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1837,7 +1850,7 @@
       <c r="I9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="21" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1845,7 +1858,7 @@
       <c r="B10" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="21" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1853,7 +1866,10 @@
       <c r="B11" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="I11" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1941,7 +1957,10 @@
       <c r="D19" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="I19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" s="25" t="s">
         <v>173</v>
       </c>
       <c r="K19" s="17" t="s">

</xml_diff>